<commit_message>
report fixed excel error
</commit_message>
<xml_diff>
--- a/public/template/Billing Statement.xlsx
+++ b/public/template/Billing Statement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RECPC2\Documents\Github\TEVES-Laravel\public\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RECPC2\OneDrive\Documents\Github\TEVES-Laravel\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50F64CEC-4BB1-4DC3-AB49-A5B8A94D2FFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D723F7C0-F355-45BD-A342-853975BEDA27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0125C2CC-56FE-4ABB-A7E4-A48064F91EF6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{0125C2CC-56FE-4ABB-A7E4-A48064F91EF6}"/>
   </bookViews>
   <sheets>
     <sheet name="May 30 2022" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
-  <si>
-    <t>TEVES GASOLINE STATION</t>
-  </si>
   <si>
     <t>San Juan, Madrid Surigao del Sur</t>
   </si>
@@ -92,6 +89,9 @@
   </si>
   <si>
     <t>Address:</t>
+  </si>
+  <si>
+    <t>G-T PETROLEUM PRODUCTS RETAILING</t>
   </si>
 </sst>
 </file>
@@ -150,7 +150,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -159,13 +159,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -212,9 +206,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -228,6 +219,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -251,16 +245,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1363345</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>252126</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>29845</xdr:rowOff>
+      <xdr:rowOff>17165</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>557530</xdr:colOff>
+      <xdr:colOff>388887</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>73025</xdr:rowOff>
+      <xdr:rowOff>141582</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -283,17 +277,23 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect t="808" b="808"/>
+        <a:srcRect/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2347595" y="29845"/>
-          <a:ext cx="2019935" cy="821055"/>
+          <a:off x="2601626" y="17165"/>
+          <a:ext cx="1607844" cy="907584"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="88900" cap="sq">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -600,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FC95511-3364-44CE-9283-D96B69225C2A}">
   <dimension ref="A1:K655"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="60" zoomScaleNormal="80" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="90" zoomScaleNormal="80" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -621,97 +621,97 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5" customHeight="1">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+    </row>
+    <row r="2" spans="1:11" ht="15" customHeight="1">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-    </row>
-    <row r="2" spans="1:11" ht="15" customHeight="1">
-      <c r="A2" s="6" t="s">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="7" t="s">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+    </row>
+    <row r="4" spans="1:11" ht="15" customHeight="1"/>
+    <row r="5" spans="1:11" ht="27" customHeight="1">
+      <c r="A5" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-    </row>
-    <row r="4" spans="1:11" ht="15" customHeight="1"/>
-    <row r="5" spans="1:11" ht="27" customHeight="1">
-      <c r="A5" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1"/>
     <row r="7" spans="1:11" ht="15.75">
       <c r="A7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+    </row>
+    <row r="8" spans="1:11" ht="15" customHeight="1">
+      <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="2" t="s">
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-    </row>
-    <row r="8" spans="1:11" ht="15" customHeight="1">
-      <c r="A8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1">
       <c r="A9" s="3"/>
@@ -727,38 +727,38 @@
       <c r="K9" s="3"/>
     </row>
     <row r="10" spans="1:11" ht="15.75">
-      <c r="A10" s="4" t="s">
-        <v>14</v>
+      <c r="A10" s="9" t="s">
+        <v>13</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="E10" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H10" s="4" t="s">
+      <c r="K10" s="9" t="s">
         <v>9</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15.75">

</xml_diff>